<commit_message>
Excel Planning Near Complete
Room Choices, Item Lists, Merchants Defined.
</commit_message>
<xml_diff>
--- a/Story and Progression.xlsx
+++ b/Story and Progression.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amosaosayande/GameDev/text-rpg-amosa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA921C54-F2C6-FD4F-B5C0-0A14ABC7A148}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CF8A67-AD55-ED48-A31D-4742C9741F61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="640" windowWidth="15600" windowHeight="19600" xr2:uid="{EFC6B3F9-5AC6-3C4C-9724-F703D2788426}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17820" windowHeight="19600" xr2:uid="{EFC6B3F9-5AC6-3C4C-9724-F703D2788426}"/>
   </bookViews>
   <sheets>
     <sheet name="Room 1" sheetId="1" r:id="rId1"/>
     <sheet name="Room 2" sheetId="5" r:id="rId2"/>
     <sheet name="Room 3" sheetId="6" r:id="rId3"/>
     <sheet name="Room 4" sheetId="7" r:id="rId4"/>
+    <sheet name="Items" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
   <si>
     <t>Text</t>
   </si>
@@ -92,11 +93,6 @@
     <t>Sub-Choices</t>
   </si>
   <si>
-    <t>If Luck &gt;= 5, you open the chest and receive all rewards. 
-If Luck = 4, you receive 20,000 Dosh
-Else HP reduced by 60%, Mimic Battle engaged.</t>
-  </si>
-  <si>
     <t>"The Holy Knight stands in defiance of all enemies"
 "Great treasure lies beyond accursed darkness"
 "Lay your tresures at the King"</t>
@@ -131,25 +127,12 @@
     <t>Ring of Favour</t>
   </si>
   <si>
-    <t>The light illuminates something on a pedestal. A closer look reveals an ornate ring.</t>
-  </si>
-  <si>
-    <t>Take Ring: Enemy Battle, ROF gives +2 Luck
-Leave Ring: No event</t>
-  </si>
-  <si>
     <t>Touch dripping liquid: Enemy ambush, Enemy has first turn
 Walk away: Enemy encounter. Turn order based on speed</t>
   </si>
   <si>
-    <t>As you approach, you see a clear liquid dripping from the ceiling. What will you do?</t>
-  </si>
-  <si>
     <t>Constant Dripping Sound 
 (Sly Spiders)</t>
-  </si>
-  <si>
-    <t>Gambler's Glasses</t>
   </si>
   <si>
     <t>NULL</t>
@@ -187,27 +170,156 @@
     <t>Crown of Illusion</t>
   </si>
   <si>
-    <t>Approach the king directly, both guards attack simultaneously
+    <t>Health Potion x5</t>
+  </si>
+  <si>
+    <t>Blessed Merchant</t>
+  </si>
+  <si>
+    <t>Cursed Merchant</t>
+  </si>
+  <si>
+    <t>Shady Merchant</t>
+  </si>
+  <si>
+    <t>Take Ring: Enemy Battle, 
+Leave Ring: No event</t>
+  </si>
+  <si>
+    <t>The light illuminates something on a pedestal. A closer look reveals an ornate ring.
+Warrior's Ring: +2 Strength, +20HP</t>
+  </si>
+  <si>
+    <t>As you approach, you see a clear liquid dripping from the ceiling. What will you do?
+Gambler's Ring: -25HP, +3 Speed, +1 LUCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You head into the next room.
+</t>
+  </si>
+  <si>
+    <t>Bloody footprints lead you further into the forest of potted plants. Where they end, a satchel lies on the floor. It is covered in blood that appears to be fresh…</t>
+  </si>
+  <si>
+    <t>Take Bag: Acquire Items
+Leave bag and return to room</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Special Effects</t>
+  </si>
+  <si>
+    <t>Health Potion</t>
+  </si>
+  <si>
+    <t>Cursed Candle</t>
+  </si>
+  <si>
+    <t>Holy Helm</t>
+  </si>
+  <si>
+    <t>Prescious Pendant</t>
+  </si>
+  <si>
+    <t>Challenge to a duel of Honour? (You must stay in the circle)
+The Guard accepts your challenge and steps forward.</t>
+  </si>
+  <si>
+    <t>Decline: Nothing
+Accept: Knight Guard Moves to circle for 1v1
+-If player flees, both Guards fight</t>
+  </si>
+  <si>
+    <t>KEY ITEM</t>
+  </si>
+  <si>
+    <t>Player Dosh</t>
+  </si>
+  <si>
+    <t>If Luck &gt;= 5, you open the chest and receive all rewards. 
+If Luck = 4, you receive 2,000 Dosh
+Else HP reduced by 60%, Mimic Battle engaged.</t>
+  </si>
+  <si>
+    <t>Restopres 35% HP</t>
+  </si>
+  <si>
+    <t>Pre-emptive Strike 100%</t>
+  </si>
+  <si>
+    <t>+10 HP each player turn</t>
+  </si>
+  <si>
+    <t>Health Potions +25HP</t>
+  </si>
+  <si>
+    <t>+2 Speed</t>
+  </si>
+  <si>
+    <t>Gambler's Ring</t>
+  </si>
+  <si>
+    <t>-20 HP, +2 Speed, +2 LUCK</t>
+  </si>
+  <si>
+    <t>+ 45% Evasion Chance</t>
+  </si>
+  <si>
+    <t>Warrior's Ring: +2 Strength, +20HP</t>
+  </si>
+  <si>
+    <t>Warrior's Ring</t>
+  </si>
+  <si>
+    <t>Fire Bomb</t>
+  </si>
+  <si>
+    <t>Deals 20 Damage</t>
+  </si>
+  <si>
+    <t>Whiskey</t>
+  </si>
+  <si>
+    <t>+1 Strength, -1 Speed</t>
+  </si>
+  <si>
+    <t>Approach the king directly, both guards attack simultaneously.
+The King Joins the fight if one dies.
 KingHP &lt; 60%, He drops his shield and two-hands his weapon</t>
   </si>
   <si>
-    <t>Health Potion x5</t>
-  </si>
-  <si>
-    <t>Blessed Merchant</t>
-  </si>
-  <si>
-    <t>Cursed Merchant</t>
-  </si>
-  <si>
-    <t>Shady Merchant</t>
+    <t>The blessed merchant offers you a deal: 25 Dosh off all items</t>
+  </si>
+  <si>
+    <t>Gambler's Ring
+Whiskey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everything comes with a condition. Will you carry a curse?
+</t>
+  </si>
+  <si>
+    <t>Health Potion
+Fire Bomb
+Royal Invitation</t>
+  </si>
+  <si>
+    <t>The unseen always plays a role in battle.</t>
+  </si>
+  <si>
+    <t>Proceed to the next room?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,6 +330,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -244,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,6 +381,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +701,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,16 +743,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -649,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -663,13 +786,13 @@
         <v>10</v>
       </c>
       <c r="E5" s="5">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -677,19 +800,19 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -700,16 +823,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -722,7 +845,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,9 +887,11 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
@@ -777,31 +902,39 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -809,17 +942,19 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -830,10 +965,14 @@
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="G7" s="4"/>
     </row>
   </sheetData>
@@ -845,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5570C7F-5902-9644-A8AB-969B845D286D}">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,9 +1022,11 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
@@ -896,39 +1037,51 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="E4" s="5">
         <v>2500</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="E5" s="5">
-        <v>3000</v>
-      </c>
-      <c r="F5" s="4"/>
+        <v>2500</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="5">
-        <v>60000</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>2500</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
@@ -937,11 +1090,15 @@
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,7 +1110,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,13 +1152,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -1009,49 +1169,59 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="109" customHeight="1" x14ac:dyDescent="0.2">
@@ -1059,19 +1229,213 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1A2E67-69EE-B74C-AFE3-B3743A9493B2}">
+  <dimension ref="B2:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>